<commit_message>
changes in exel file for lab2 and lab3,4,5 added
</commit_message>
<xml_diff>
--- a/lab2/lab2.xlsx
+++ b/lab2/lab2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ДенисВладимирович\kszi\lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD91750-4538-44A8-BC16-468807BDD61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8DAFDF-A890-469E-95D3-63FAB95D0E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1ший спосіб" sheetId="1" r:id="rId1"/>
+    <sheet name="2гий спосіб" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Швидкодія доступу до ДМЗ</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Захист від НСД внутрішньої мережі</t>
   </si>
@@ -51,22 +49,33 @@
     <t>Легкість адміністрування</t>
   </si>
   <si>
-    <t>Сума</t>
+    <t>швидкість доступу до ДМЗ</t>
   </si>
   <si>
-    <t>Вага</t>
+    <t>сума по рядку</t>
+  </si>
+  <si>
+    <t>вага</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -113,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -149,43 +158,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{2990751C-2081-4086-865C-1BE7E621BA63}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{FAAB1D6D-B97C-44FC-A0DD-924451F56CD0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -465,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,156 +504,144 @@
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <f>1/4</f>
+      <c r="C2" s="2">
         <v>0.25</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.5</v>
-      </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>0.33</v>
       </c>
       <c r="E2" s="2">
         <v>3</v>
       </c>
       <c r="F2" s="1">
-        <f>SUM(A2:E2)</f>
-        <v>6.75</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1">
-        <f>F2/$F$7</f>
-        <v>0.16695523126391293</v>
+        <v>7.58</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12">
         <v>4</v>
       </c>
-      <c r="B3" s="12">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
-        <v>6</v>
-      </c>
       <c r="E3" s="2">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F6" si="0">SUM(A3:E3)</f>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G7" si="1">F3/$F$7</f>
-        <v>0.39574573336631214</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
-        <v>0.6</v>
-      </c>
       <c r="C4" s="11">
+        <v>0.33</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>0.28691565669057628</v>
+        <v>11.33</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
         <v>0.33</v>
       </c>
-      <c r="B5" s="6">
-        <v>0.12</v>
-      </c>
       <c r="C5" s="2">
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>3.65</v>
-      </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
-        <v>9.0279495424189962E-2</v>
+        <v>7.58</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
         <v>0.33</v>
       </c>
-      <c r="B6" s="6">
-        <v>0.2</v>
-      </c>
       <c r="C6" s="2">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="D6" s="3">
-        <v>0.7</v>
+        <v>0.33</v>
       </c>
       <c r="E6" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>2.4299999999999997</v>
-      </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>6.010388325500865E-2</v>
+        <v>2.4900000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -634,13 +650,84 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="5">
-        <f>SUM(F2:F6)</f>
-        <v>40.43</v>
-      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="1">
-        <f t="shared" si="1"/>
+        <v>40.229999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA47CB53-0D20-43E8-BAA1-6A4D67C433F1}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>2.8769999999999998</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0.16525934861278649</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>4.8890000000000002</v>
+      </c>
+      <c r="B3" s="14">
+        <v>0.2808317536906198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>4.7450000000000001</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0.27256017002699756</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>3.8980000000000001</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0.22390717444999714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
         <v>1</v>
+      </c>
+      <c r="B6" s="14">
+        <v>5.7441553219599061E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>17.408999999999999</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1.0000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>